<commit_message>
Update consolidated log file
Signed-off-by: Sanjiv Krish <sanjiv436.k@gmail.com>
</commit_message>
<xml_diff>
--- a/logs/EC - Consolidated log.xlsx
+++ b/logs/EC - Consolidated log.xlsx
@@ -1467,97 +1467,97 @@
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
     </row>
-    <row r="163">
-      <c r="A163" s="1" t="s">
+    <row r="112">
+      <c r="A112" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="165">
-      <c r="A165" s="1" t="s">
+    <row r="114">
+      <c r="A114" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B165" s="1" t="s">
+      <c r="B114" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C165" s="1" t="s">
+      <c r="C114" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="166">
-      <c r="A166" s="1">
+    <row r="115">
+      <c r="A115" s="1">
         <v>8.0</v>
       </c>
-      <c r="B166" s="1">
+      <c r="B115" s="1">
         <v>103.7</v>
       </c>
-      <c r="C166" s="1">
-        <v>88.04</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" s="1">
+      <c r="C115" s="1">
+        <v>67.79</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1">
         <v>16.0</v>
       </c>
-      <c r="B167" s="1">
+      <c r="B116" s="1">
         <v>132.49</v>
       </c>
-      <c r="C167" s="1">
-        <v>141.1</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" s="1">
+      <c r="C116" s="1">
+        <v>108.4</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1">
         <v>32.0</v>
       </c>
-      <c r="B168" s="1">
+      <c r="B117" s="1">
         <v>256.32</v>
       </c>
-      <c r="C168" s="1">
-        <v>383.26</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" s="1">
+      <c r="C117" s="1">
+        <v>214.54</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1">
         <v>64.0</v>
       </c>
-      <c r="B169" s="1">
+      <c r="B118" s="1">
         <v>566.42</v>
       </c>
-      <c r="C169" s="1">
-        <v>853.56</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" s="1">
+      <c r="C118" s="1">
+        <v>453.34</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1">
         <v>128.0</v>
       </c>
-      <c r="B170" s="1">
+      <c r="B119" s="1">
         <v>2796.3</v>
       </c>
-      <c r="C170" s="1">
-        <v>2720.21</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" s="1">
+      <c r="C119" s="1">
+        <v>1009.34</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1">
         <v>256.0</v>
       </c>
-      <c r="B171" s="1">
+      <c r="B120" s="1">
         <v>5418.26</v>
       </c>
-      <c r="C171" s="1">
-        <v>4601.26</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" s="1">
+      <c r="C120" s="1">
+        <v>2752.25</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1">
         <v>512.0</v>
       </c>
-      <c r="B172" s="1">
+      <c r="B121" s="1">
         <v>9708.95</v>
       </c>
-      <c r="C172" s="1">
-        <v>13277.68</v>
+      <c r="C121" s="1">
+        <v>8556.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>